<commit_message>
Actualización de excel para distribución de tareas
</commit_message>
<xml_diff>
--- a/EDTCLUB.xlsx
+++ b/EDTCLUB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neyth\Escritorio\pclubmecatronica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neyth\Escritorio\CMMecatronica\cmweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF25FBB-F195-4BD7-844B-5E566C45B788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC12243-7B79-4D01-977F-84413E88C619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>WBS (Work Breakdown Structure) o EDT (Estructura de Descomposición del Trabajo)</t>
   </si>
@@ -196,6 +196,54 @@
   </si>
   <si>
     <t>Sitio Web Club de Mecatrónica</t>
+  </si>
+  <si>
+    <t>Inventario Control Page</t>
+  </si>
+  <si>
+    <t>Componente de visualización de materiales disponibles</t>
+  </si>
+  <si>
+    <t>sistema de préstamo de materiales</t>
+  </si>
+  <si>
+    <t>Neythan</t>
+  </si>
+  <si>
+    <t>David &amp; Angie</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Darly</t>
+  </si>
+  <si>
+    <t>Arom</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Arom &amp; Carlos</t>
+  </si>
+  <si>
+    <t>Diseño de Mockup para Panel de Control de cada Usuario</t>
+  </si>
+  <si>
+    <t>Diseño de Mockup para portal de publicación de proyectos</t>
+  </si>
+  <si>
+    <t>Diseño de Mockup para panel de administración directiva</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Angie</t>
+  </si>
+  <si>
+    <t>Diana</t>
   </si>
 </sst>
 </file>
@@ -234,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,8 +331,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -369,11 +423,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -394,68 +485,108 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A10" activeCellId="3" sqref="A16:B18 A6:B6 A7:B7 A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -761,160 +892,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="5.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2"/>
       <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="24"/>
+      <c r="G7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="2"/>
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="17" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="2"/>
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="27"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="2"/>
       <c r="D11" s="4" t="s">
         <v>33</v>
@@ -923,10 +1054,10 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="2"/>
       <c r="D12" s="4" t="s">
         <v>34</v>
@@ -937,10 +1068,10 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="14"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="2"/>
       <c r="D13" s="4" t="s">
         <v>35</v>
@@ -951,10 +1082,10 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="2"/>
       <c r="D14" s="4" t="s">
         <v>36</v>
@@ -979,8 +1110,10 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="22"/>
       <c r="C16" s="2"/>
       <c r="D16" s="4" t="s">
         <v>38</v>
@@ -991,20 +1124,24 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="21" t="s">
+      <c r="A17" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="22"/>
       <c r="C18" s="2"/>
       <c r="D18" s="4" t="s">
         <v>40</v>
@@ -1015,8 +1152,8 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="2"/>
       <c r="D19" s="4" t="s">
         <v>41</v>
@@ -1053,10 +1190,10 @@
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="21"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1077,42 +1214,46 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="4"/>
+      <c r="C24" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="29"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="21"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="C27" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="27"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1123,7 +1264,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1131,20 +1272,34 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C26:D26"/>
+  <mergeCells count="35">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G8:H8"/>
@@ -1160,12 +1315,15 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1174,13 +1332,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:C1"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1196,10 +1354,10 @@
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="6" t="s">
         <v>28</v>
       </c>
@@ -1207,384 +1365,552 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8">
+    <row r="2" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="45">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="45">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="45">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="45">
         <v>5</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="27"/>
-    </row>
-    <row r="3" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="10">
+      <c r="B6" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="45">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="45">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8">
-        <v>6</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="8">
+      <c r="C8" s="27"/>
+      <c r="D8" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="45">
         <v>8</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8">
-        <v>9</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="10">
+        <v>50</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="8">
-        <v>10</v>
+      <c r="A10" s="45">
+        <v>9</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="10">
+        <v>13</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8">
-        <v>11</v>
+      <c r="A11" s="45">
+        <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="8">
+        <v>16</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="45">
+        <v>11</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="45">
         <v>12</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8">
+      <c r="B13" s="2"/>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="45">
         <v>13</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="8">
-        <v>14</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="10">
+        <v>34</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="8">
-        <v>15</v>
+      <c r="A15" s="45">
+        <v>14</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="10">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="9">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="8">
-        <v>16</v>
+      <c r="A16" s="45">
+        <v>15</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="8">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="45">
+        <v>16</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="27">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="D17" s="35"/>
+      <c r="E17" s="9">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="8">
+      <c r="A18" s="45">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="45">
         <v>18</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="8">
+      <c r="B19" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="45">
         <v>19</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="8">
-        <v>21</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="27"/>
-    </row>
-    <row r="21" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="8">
-        <v>22</v>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="45">
+        <v>20</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="8">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="45">
+        <v>21</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="45">
+        <v>22</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="45">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="45">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="39"/>
+      <c r="E25" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="45">
+        <v>25</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="45">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="45">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="45">
+        <v>28</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="45">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="45">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="10">
+      <c r="D31" s="37"/>
+      <c r="E31" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="8">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="45">
+        <v>31</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="45">
+        <v>32</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="9">
         <v>25</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="8">
-        <v>26</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="10">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="45">
+        <v>33</v>
+      </c>
+      <c r="B34" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="8">
+      <c r="C34" s="24"/>
+      <c r="D34" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="45">
+        <v>34</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="24"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="45">
+        <v>35</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="45">
+        <v>36</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="45">
+        <v>37</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D39" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="29.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="8">
-        <v>31</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="8">
-        <v>33</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="8">
-        <v>34</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="28">
-        <f>SUM(E2:E29)</f>
-        <v>192</v>
+      <c r="E39" s="12">
+        <f>SUM(E2:E38)</f>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B25:C25"/>
+  <mergeCells count="29">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D32:D33"/>
     <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>